<commit_message>
Model Updates, Added Upload Code
</commit_message>
<xml_diff>
--- a/Classes/ConceptualDomain.xlsx
+++ b/Classes/ConceptualDomain.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Geothermal_DOE\ContentModelsDevelopment\Linked Data Registry\Registry Classes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Geothermal_DOE\ContentModelsDevelopment\Linked Data Registry\Classes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13785"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13788"/>
   </bookViews>
   <sheets>
     <sheet name="ConceptualDomain" sheetId="1" r:id="rId1"/>
@@ -95,10 +95,10 @@
     <t>dct:description</t>
   </si>
   <si>
-    <t>skos:prefLabel</t>
-  </si>
-  <si>
     <t>URI</t>
+  </si>
+  <si>
+    <t>dcdtr:domainName</t>
   </si>
 </sst>
 </file>
@@ -469,25 +469,26 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="22" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>22</v>
@@ -499,9 +500,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
-        <f>"class/conceptual-domain/"&amp;LOWER(SUBSTITUTE(B2," ", "-"))</f>
+        <f t="shared" ref="A2:A11" si="0">"class/conceptual-domain/"&amp;LOWER(SUBSTITUTE(B2," ", "-"))</f>
         <v>class/conceptual-domain/software-environments</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -511,9 +512,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
-        <f>"class/conceptual-domain/"&amp;LOWER(SUBSTITUTE(B3," ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>class/conceptual-domain/units-of-measurement</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -523,9 +524,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
-        <f>"class/conceptual-domain/"&amp;LOWER(SUBSTITUTE(B4," ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>class/conceptual-domain/magnitude-of-power</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -535,9 +536,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
-        <f>"class/conceptual-domain/"&amp;LOWER(SUBSTITUTE(B5," ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>class/conceptual-domain/degrees-of-latitude</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -547,9 +548,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
-        <f>"class/conceptual-domain/"&amp;LOWER(SUBSTITUTE(B6," ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>class/conceptual-domain/degrees-of-longitude</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -559,9 +560,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
-        <f>"class/conceptual-domain/"&amp;LOWER(SUBSTITUTE(B7," ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>class/conceptual-domain/location-on-earth</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -571,9 +572,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
-        <f>"class/conceptual-domain/"&amp;LOWER(SUBSTITUTE(B8," ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>class/conceptual-domain/agents</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -583,9 +584,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="str">
-        <f>"class/conceptual-domain/"&amp;LOWER(SUBSTITUTE(B9," ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>class/conceptual-domain/unique-bitstream</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -595,9 +596,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="str">
-        <f>"class/conceptual-domain/"&amp;LOWER(SUBSTITUTE(B10," ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>class/conceptual-domain/solid-material</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -607,9 +608,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="114" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="110.4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="str">
-        <f>"class/conceptual-domain/"&amp;LOWER(SUBSTITUTE(B11," ", "-"))</f>
+        <f t="shared" si="0"/>
         <v>class/conceptual-domain/porous-material</v>
       </c>
       <c r="B11" s="2" t="s">

</xml_diff>